<commit_message>
made full weight set for admin_for_testing.xlsx
and updated tests to work with the full set.
</commit_message>
<xml_diff>
--- a/tests/samples/admin_for_testing.xlsx
+++ b/tests/samples/admin_for_testing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\tests\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebecca.hawke\PycharmProjects\Mass-Circular-Weighing\tests\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B85673E-C974-4E6C-B330-CE883AEFA7EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D15546E-CC5A-47CC-BB76-95A0E332C263}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F7F7C31D-9B21-4E63-BF52-B7D512313953}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15460" xr2:uid="{F7F7C31D-9B21-4E63-BF52-B7D512313953}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
   <si>
     <t>Client</t>
   </si>
@@ -226,12 +226,6 @@
     <t>2d</t>
   </si>
   <si>
-    <t>1 kg to 1 g weight set</t>
-  </si>
-  <si>
-    <t>1 kg to 1 g 5-2-2-1 weight set</t>
-  </si>
-  <si>
     <t>Weights are housed in a wooden box with label GSW3240</t>
   </si>
   <si>
@@ -257,6 +251,48 @@
   </si>
   <si>
     <t>u_dens</t>
+  </si>
+  <si>
+    <t>1 kg to 1 mg 5-2-2-1 weight set</t>
+  </si>
+  <si>
+    <t>1 kg to 1 mg weight set</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.2d</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>0.02d</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.005</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>0.002d</t>
+  </si>
+  <si>
+    <t>0.001</t>
   </si>
 </sst>
 </file>
@@ -338,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -393,6 +429,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -725,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AB355D-84BE-43AB-B2BC-CDE069094A48}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:H7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -745,10 +784,10 @@
       <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="25"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -768,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>50</v>
@@ -776,11 +815,11 @@
       <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="E3" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
@@ -821,68 +860,68 @@
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="24"/>
+      <c r="B7" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="25"/>
       <c r="D7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="24"/>
+      <c r="B8" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="25"/>
       <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -891,16 +930,16 @@
         <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="18"/>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="27"/>
+      <c r="F11" s="28"/>
       <c r="G11" s="17" t="s">
         <v>46</v>
       </c>
@@ -914,16 +953,16 @@
       <c r="A13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="26"/>
+      <c r="C13" s="27"/>
       <c r="D13" t="s">
         <v>29</v>
       </c>
       <c r="E13">
         <f>COUNT(B15:B90)</f>
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>47</v>
@@ -931,7 +970,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>17</v>
@@ -949,7 +988,7 @@
         <v>11</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H14" t="s">
         <v>21</v>
@@ -1137,108 +1176,156 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="14"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="7"/>
+      <c r="A28" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="21"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="7"/>
+      <c r="A29" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C29" s="21"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="14"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="7"/>
+      <c r="A30" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C30" s="21"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="7"/>
+      <c r="A31" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C31" s="21"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="14"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="7"/>
+      <c r="A32" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="C32" s="21"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="14"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="7"/>
+      <c r="A33" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="C33" s="21"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="14"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="7"/>
+      <c r="A34" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="C34" s="21"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="14"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="7"/>
+      <c r="A35" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C35" s="21"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="14"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="7"/>
+      <c r="A36" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C36" s="21"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="14"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="7"/>
+      <c r="A37" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="C37" s="21"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="14"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="7"/>
+      <c r="A38" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="C38" s="21"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="14"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="7"/>
+      <c r="A39" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C39" s="23"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>

</xml_diff>